<commit_message>
Updated kīhai ki Accidentally ran 'tidy up html' on all the K's hopefully won't matter...
</commit_message>
<xml_diff>
--- a/head_words_excel/hpk_headwords_k.xlsx
+++ b/head_words_excel/hpk_headwords_k.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="141"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="82"/>
   </bookViews>
   <sheets>
     <sheet name="177" sheetId="1" state="visible" r:id="rId2"/>
@@ -2915,7 +2915,7 @@
     <t>kīhai</t>
   </si>
   <si>
-    <t>kīhai ki</t>
+    <t>kīhai ki . . .</t>
   </si>
   <si>
     <t>kihakiha</t>
@@ -11708,8 +11708,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24781,8 +24781,8 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>